<commit_message>
Added qPCR instrument type to migration and library QC template.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_QC_v4_1_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_QC_v4_1_0.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="428">
   <si>
     <t xml:space="preserve">Library QC Template</t>
   </si>
@@ -144,64 +144,67 @@
     <t xml:space="preserve">Agarose Gel</t>
   </si>
   <si>
+    <t xml:space="preserve">qPCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double stranded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step complete - Move to next step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TapeStation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qubit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single stranded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample failed - Remove sample from study workflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NanoDrop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignore workflow - Do not register as part of a workflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caliper LabChip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tecan Absorbance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BioAnalyzer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A08</t>
+  </si>
+  <si>
     <t xml:space="preserve">PicoGreen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Double stranded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step complete - Move to next step</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Failed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TapeStation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qubit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single stranded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample failed - Remove sample from study workflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NanoDrop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ignore workflow - Do not register as part of a workflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caliper LabChip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tecan Absorbance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BioAnalyzer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A08</t>
   </si>
   <si>
     <t xml:space="preserve">A09</t>
@@ -1340,7 +1343,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1393,6 +1396,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1548,7 +1557,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1673,6 +1682,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1756,7 +1769,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.88"/>
@@ -1764,7 +1777,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="0" width="18.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.38"/>
@@ -6764,7 +6777,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N8:N103" type="list">
-      <formula1>Index!$E$2:$E$8</formula1>
+      <formula1>Index!$E$2:$E$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G8:G103" type="list">
@@ -6796,22 +6809,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K586"/>
+  <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="43.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="55.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6998,7 +7011,7 @@
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="31" t="s">
         <v>36</v>
       </c>
       <c r="F8" s="29"/>
@@ -7016,2154 +7029,2157 @@
         <v>50</v>
       </c>
       <c r="C9" s="29"/>
+      <c r="E9" s="31" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C10" s="29"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C11" s="29"/>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C12" s="29"/>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C13" s="29"/>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C14" s="29"/>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="29" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="29" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="29" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="29" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="29" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="29" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="29" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="29" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="29" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="29" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="29" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="29" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B57" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B58" s="29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="29" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B59" s="29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="29" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B60" s="29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="29" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B61" s="29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="29" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B62" s="29" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="29" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B63" s="29" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="29" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B64" s="29" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="29" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B65" s="29" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="29" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B66" s="29" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="29" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B67" s="29" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="29" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B68" s="29" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="29" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B69" s="29" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="29" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B70" s="29" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="29" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B71" s="29" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="29" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B72" s="29" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="29" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B73" s="29" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B74" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="29" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B75" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B76" s="29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="29" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B77" s="29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="29" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B78" s="29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="29" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B79" s="29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="29" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B80" s="29" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="29" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B81" s="29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="29" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B82" s="29" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="29" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B83" s="29" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="29" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B84" s="29" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="29" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B85" s="29" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="29" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B86" s="29" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="29" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B87" s="29" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="29" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B88" s="29" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="29" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B89" s="29" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="29" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B90" s="29" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B91" s="29" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="29" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B92" s="29" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="29" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B93" s="29" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="29" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B94" s="29" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="29" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B95" s="29" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="29" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B96" s="29" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="29" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B97" s="29" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="29" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="29" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="29" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="29" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="29" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="29" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="29" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="29" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="29" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="29" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="29" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="29" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="29" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="29" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="29" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="29" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="29" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="29" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="29" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="29" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="29" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="29" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="29" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="29" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="29" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="29" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="29" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="29" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="29" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="29" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="29" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="29" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="29" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="29" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="29" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="29" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="29" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="29" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="29" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="29" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="29" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="29" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="29" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="29" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="29" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="29" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="29" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="29" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="29" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="29" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="29" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="29" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="29" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="29" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="29" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="29" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="29" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="29" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="29" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="29" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="29" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="29" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="29" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="29" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="29" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="29" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="29" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="29" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="29" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="29" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="29" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="29" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="29" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="29" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="29" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="29" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="29" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="29" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="29" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="29" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="29" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="29" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="29" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="29" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="29" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="29" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="29" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="29" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="29" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="29" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="29" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="29" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="29" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="29" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="29" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="29" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B201" s="29" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B202" s="29" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B203" s="29" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B204" s="29" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B205" s="29" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B206" s="29" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B207" s="29" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B208" s="29" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B209" s="29" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B210" s="29" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B211" s="29" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B212" s="29" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B213" s="29" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B214" s="29" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B215" s="29" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B216" s="29" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B217" s="29" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B218" s="29" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B219" s="29" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B220" s="29" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B221" s="29" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B222" s="29" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B223" s="29" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B224" s="29" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B225" s="29" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B226" s="29" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B227" s="29" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B228" s="29" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B229" s="29" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B230" s="29" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B231" s="29" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B232" s="29" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B233" s="29" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B234" s="29" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B235" s="29" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B236" s="29" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B237" s="29" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B238" s="29" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B239" s="29" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B240" s="29" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B241" s="29" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B242" s="29" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B243" s="29" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B244" s="29" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B245" s="29" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B246" s="29" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B247" s="29" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B248" s="29" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B249" s="29" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B250" s="29" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B251" s="29" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B252" s="29" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B253" s="29" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B254" s="29" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B255" s="29" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B256" s="29" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B257" s="29" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B258" s="29" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B259" s="29" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B260" s="29" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B261" s="29" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B262" s="29" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B263" s="29" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B264" s="29" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B265" s="29" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B266" s="29" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B267" s="29" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B268" s="29" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B269" s="29" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B270" s="29" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B271" s="29" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B272" s="29" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B273" s="29" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B274" s="29" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B275" s="29" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B276" s="29" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B277" s="29" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B278" s="29" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B279" s="29" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B280" s="29" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B281" s="29" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B282" s="29" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B283" s="29" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B284" s="29" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B285" s="29" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B286" s="29" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B287" s="29" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B288" s="29" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B289" s="29" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B290" s="29" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B291" s="29" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B292" s="29" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B293" s="29" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B294" s="29" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B295" s="29" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B296" s="29" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B297" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B298" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B299" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B300" s="29" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B301" s="29" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B302" s="29" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B303" s="29" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B304" s="29" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B305" s="29" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B306" s="29" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B307" s="29" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B308" s="29" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B309" s="29" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B310" s="29" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B311" s="29" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B312" s="29" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B313" s="29" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B314" s="29" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B315" s="29" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B316" s="29" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B317" s="29" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B318" s="29" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B319" s="29" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B320" s="29" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B321" s="29" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B322" s="29" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B323" s="29" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B324" s="29" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B325" s="29" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B326" s="29" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B327" s="29" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B328" s="29" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B329" s="29" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B330" s="29" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B331" s="29" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B332" s="29" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B333" s="29" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B334" s="29" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B335" s="29" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B336" s="29" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B337" s="29" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B338" s="29" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B339" s="29" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B340" s="29" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B341" s="29" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B342" s="29" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B343" s="29" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B344" s="29" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B345" s="29" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B346" s="29" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B347" s="29" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B348" s="29" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B349" s="29" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B350" s="29" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B351" s="29" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B352" s="29" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B353" s="29" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B354" s="29" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B355" s="29" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B356" s="29" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B357" s="29" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B358" s="29" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B359" s="29" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B360" s="29" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B361" s="29" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B362" s="29" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B363" s="29" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B364" s="29" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B365" s="29" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B366" s="29" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B367" s="29" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B368" s="29" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B369" s="29" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B370" s="29" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B371" s="29" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B372" s="29" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B373" s="29" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B374" s="29" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B375" s="29" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B376" s="29" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B377" s="29" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B378" s="29" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B379" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B380" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B381" s="29" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B382" s="29" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B383" s="29" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B384" s="29" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B385" s="29" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Start modification for Normalization Library removal and changes to pooling.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_QC_v4_1_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_QC_v4_1_0.xlsx
@@ -27,7 +27,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>UFG</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="E7" authorId="0">
@@ -1343,7 +1343,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1396,12 +1396,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1662,6 +1656,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1680,10 +1678,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1769,7 +1763,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.88"/>
@@ -1882,7 +1876,7 @@
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
-      <c r="K8" s="15" t="str">
+      <c r="K8" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E8),AND(OR(ISBLANK(G8),ISBLANK(H8),ISBLANK(I8)),ISBLANK(J8))),"",IF(ISBLANK(J8),(E8-F8)*I8*H8*INDIRECT(SUBSTITUTE(G8," ","_"))/1000000,(E8-F8)*J8))</f>
         <v/>
       </c>
@@ -1905,7 +1899,7 @@
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
-      <c r="K9" s="15" t="str">
+      <c r="K9" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E9),AND(OR(ISBLANK(G9),ISBLANK(H9),ISBLANK(I9)),ISBLANK(J9))),"",IF(ISBLANK(J9),(E9-F9)*I9*H9*INDIRECT(SUBSTITUTE(G9," ","_"))/1000000,(E9-F9)*J9))</f>
         <v/>
       </c>
@@ -1928,7 +1922,7 @@
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
-      <c r="K10" s="15" t="str">
+      <c r="K10" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E10),AND(OR(ISBLANK(G10),ISBLANK(H10),ISBLANK(I10)),ISBLANK(J10))),"",IF(ISBLANK(J10),(E10-F10)*I10*H10*INDIRECT(SUBSTITUTE(G10," ","_"))/1000000,(E10-F10)*J10))</f>
         <v/>
       </c>
@@ -1951,7 +1945,7 @@
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
-      <c r="K11" s="15" t="str">
+      <c r="K11" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E11),AND(OR(ISBLANK(G11),ISBLANK(H11),ISBLANK(I11)),ISBLANK(J11))),"",IF(ISBLANK(J11),(E11-F11)*I11*H11*INDIRECT(SUBSTITUTE(G11," ","_"))/1000000,(E11-F11)*J11))</f>
         <v/>
       </c>
@@ -1974,7 +1968,7 @@
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
-      <c r="K12" s="15" t="str">
+      <c r="K12" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E12),AND(OR(ISBLANK(G12),ISBLANK(H12),ISBLANK(I12)),ISBLANK(J12))),"",IF(ISBLANK(J12),(E12-F12)*I12*H12*INDIRECT(SUBSTITUTE(G12," ","_"))/1000000,(E12-F12)*J12))</f>
         <v/>
       </c>
@@ -1997,7 +1991,7 @@
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
-      <c r="K13" s="15" t="str">
+      <c r="K13" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E13),AND(OR(ISBLANK(G13),ISBLANK(H13),ISBLANK(I13)),ISBLANK(J13))),"",IF(ISBLANK(J13),(E13-F13)*I13*H13*INDIRECT(SUBSTITUTE(G13," ","_"))/1000000,(E13-F13)*J13))</f>
         <v/>
       </c>
@@ -2020,7 +2014,7 @@
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="15" t="str">
+      <c r="K14" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E14),AND(OR(ISBLANK(G14),ISBLANK(H14),ISBLANK(I14)),ISBLANK(J14))),"",IF(ISBLANK(J14),(E14-F14)*I14*H14*INDIRECT(SUBSTITUTE(G14," ","_"))/1000000,(E14-F14)*J14))</f>
         <v/>
       </c>
@@ -2043,7 +2037,7 @@
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="15" t="str">
+      <c r="K15" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E15),AND(OR(ISBLANK(G15),ISBLANK(H15),ISBLANK(I15)),ISBLANK(J15))),"",IF(ISBLANK(J15),(E15-F15)*I15*H15*INDIRECT(SUBSTITUTE(G15," ","_"))/1000000,(E15-F15)*J15))</f>
         <v/>
       </c>
@@ -2066,7 +2060,7 @@
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
-      <c r="K16" s="15" t="str">
+      <c r="K16" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E16),AND(OR(ISBLANK(G16),ISBLANK(H16),ISBLANK(I16)),ISBLANK(J16))),"",IF(ISBLANK(J16),(E16-F16)*I16*H16*INDIRECT(SUBSTITUTE(G16," ","_"))/1000000,(E16-F16)*J16))</f>
         <v/>
       </c>
@@ -2089,7 +2083,7 @@
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
-      <c r="K17" s="15" t="str">
+      <c r="K17" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E17),AND(OR(ISBLANK(G17),ISBLANK(H17),ISBLANK(I17)),ISBLANK(J17))),"",IF(ISBLANK(J17),(E17-F17)*I17*H17*INDIRECT(SUBSTITUTE(G17," ","_"))/1000000,(E17-F17)*J17))</f>
         <v/>
       </c>
@@ -2112,7 +2106,7 @@
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
-      <c r="K18" s="15" t="str">
+      <c r="K18" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E18),AND(OR(ISBLANK(G18),ISBLANK(H18),ISBLANK(I18)),ISBLANK(J18))),"",IF(ISBLANK(J18),(E18-F18)*I18*H18*INDIRECT(SUBSTITUTE(G18," ","_"))/1000000,(E18-F18)*J18))</f>
         <v/>
       </c>
@@ -2135,7 +2129,7 @@
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
-      <c r="K19" s="15" t="str">
+      <c r="K19" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E19),AND(OR(ISBLANK(G19),ISBLANK(H19),ISBLANK(I19)),ISBLANK(J19))),"",IF(ISBLANK(J19),(E19-F19)*I19*H19*INDIRECT(SUBSTITUTE(G19," ","_"))/1000000,(E19-F19)*J19))</f>
         <v/>
       </c>
@@ -2158,7 +2152,7 @@
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
-      <c r="K20" s="15" t="str">
+      <c r="K20" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E20),AND(OR(ISBLANK(G20),ISBLANK(H20),ISBLANK(I20)),ISBLANK(J20))),"",IF(ISBLANK(J20),(E20-F20)*I20*H20*INDIRECT(SUBSTITUTE(G20," ","_"))/1000000,(E20-F20)*J20))</f>
         <v/>
       </c>
@@ -2181,7 +2175,7 @@
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
-      <c r="K21" s="15" t="str">
+      <c r="K21" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E21),AND(OR(ISBLANK(G21),ISBLANK(H21),ISBLANK(I21)),ISBLANK(J21))),"",IF(ISBLANK(J21),(E21-F21)*I21*H21*INDIRECT(SUBSTITUTE(G21," ","_"))/1000000,(E21-F21)*J21))</f>
         <v/>
       </c>
@@ -2204,7 +2198,7 @@
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
-      <c r="K22" s="15" t="str">
+      <c r="K22" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E22),AND(OR(ISBLANK(G22),ISBLANK(H22),ISBLANK(I22)),ISBLANK(J22))),"",IF(ISBLANK(J22),(E22-F22)*I22*H22*INDIRECT(SUBSTITUTE(G22," ","_"))/1000000,(E22-F22)*J22))</f>
         <v/>
       </c>
@@ -2227,7 +2221,7 @@
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
-      <c r="K23" s="15" t="str">
+      <c r="K23" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E23),AND(OR(ISBLANK(G23),ISBLANK(H23),ISBLANK(I23)),ISBLANK(J23))),"",IF(ISBLANK(J23),(E23-F23)*I23*H23*INDIRECT(SUBSTITUTE(G23," ","_"))/1000000,(E23-F23)*J23))</f>
         <v/>
       </c>
@@ -2250,7 +2244,7 @@
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
-      <c r="K24" s="15" t="str">
+      <c r="K24" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E24),AND(OR(ISBLANK(G24),ISBLANK(H24),ISBLANK(I24)),ISBLANK(J24))),"",IF(ISBLANK(J24),(E24-F24)*I24*H24*INDIRECT(SUBSTITUTE(G24," ","_"))/1000000,(E24-F24)*J24))</f>
         <v/>
       </c>
@@ -2273,7 +2267,7 @@
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
-      <c r="K25" s="15" t="str">
+      <c r="K25" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E25),AND(OR(ISBLANK(G25),ISBLANK(H25),ISBLANK(I25)),ISBLANK(J25))),"",IF(ISBLANK(J25),(E25-F25)*I25*H25*INDIRECT(SUBSTITUTE(G25," ","_"))/1000000,(E25-F25)*J25))</f>
         <v/>
       </c>
@@ -2296,7 +2290,7 @@
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
-      <c r="K26" s="15" t="str">
+      <c r="K26" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E26),AND(OR(ISBLANK(G26),ISBLANK(H26),ISBLANK(I26)),ISBLANK(J26))),"",IF(ISBLANK(J26),(E26-F26)*I26*H26*INDIRECT(SUBSTITUTE(G26," ","_"))/1000000,(E26-F26)*J26))</f>
         <v/>
       </c>
@@ -2319,7 +2313,7 @@
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
-      <c r="K27" s="15" t="str">
+      <c r="K27" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E27),AND(OR(ISBLANK(G27),ISBLANK(H27),ISBLANK(I27)),ISBLANK(J27))),"",IF(ISBLANK(J27),(E27-F27)*I27*H27*INDIRECT(SUBSTITUTE(G27," ","_"))/1000000,(E27-F27)*J27))</f>
         <v/>
       </c>
@@ -2342,7 +2336,7 @@
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
-      <c r="K28" s="15" t="str">
+      <c r="K28" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E28),AND(OR(ISBLANK(G28),ISBLANK(H28),ISBLANK(I28)),ISBLANK(J28))),"",IF(ISBLANK(J28),(E28-F28)*I28*H28*INDIRECT(SUBSTITUTE(G28," ","_"))/1000000,(E28-F28)*J28))</f>
         <v/>
       </c>
@@ -2365,7 +2359,7 @@
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
-      <c r="K29" s="15" t="str">
+      <c r="K29" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E29),AND(OR(ISBLANK(G29),ISBLANK(H29),ISBLANK(I29)),ISBLANK(J29))),"",IF(ISBLANK(J29),(E29-F29)*I29*H29*INDIRECT(SUBSTITUTE(G29," ","_"))/1000000,(E29-F29)*J29))</f>
         <v/>
       </c>
@@ -2388,7 +2382,7 @@
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
-      <c r="K30" s="15" t="str">
+      <c r="K30" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E30),AND(OR(ISBLANK(G30),ISBLANK(H30),ISBLANK(I30)),ISBLANK(J30))),"",IF(ISBLANK(J30),(E30-F30)*I30*H30*INDIRECT(SUBSTITUTE(G30," ","_"))/1000000,(E30-F30)*J30))</f>
         <v/>
       </c>
@@ -2411,7 +2405,7 @@
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
-      <c r="K31" s="15" t="str">
+      <c r="K31" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E31),AND(OR(ISBLANK(G31),ISBLANK(H31),ISBLANK(I31)),ISBLANK(J31))),"",IF(ISBLANK(J31),(E31-F31)*I31*H31*INDIRECT(SUBSTITUTE(G31," ","_"))/1000000,(E31-F31)*J31))</f>
         <v/>
       </c>
@@ -2434,7 +2428,7 @@
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
-      <c r="K32" s="15" t="str">
+      <c r="K32" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E32),AND(OR(ISBLANK(G32),ISBLANK(H32),ISBLANK(I32)),ISBLANK(J32))),"",IF(ISBLANK(J32),(E32-F32)*I32*H32*INDIRECT(SUBSTITUTE(G32," ","_"))/1000000,(E32-F32)*J32))</f>
         <v/>
       </c>
@@ -2457,7 +2451,7 @@
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
-      <c r="K33" s="15" t="str">
+      <c r="K33" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E33),AND(OR(ISBLANK(G33),ISBLANK(H33),ISBLANK(I33)),ISBLANK(J33))),"",IF(ISBLANK(J33),(E33-F33)*I33*H33*INDIRECT(SUBSTITUTE(G33," ","_"))/1000000,(E33-F33)*J33))</f>
         <v/>
       </c>
@@ -2480,7 +2474,7 @@
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
-      <c r="K34" s="15" t="str">
+      <c r="K34" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E34),AND(OR(ISBLANK(G34),ISBLANK(H34),ISBLANK(I34)),ISBLANK(J34))),"",IF(ISBLANK(J34),(E34-F34)*I34*H34*INDIRECT(SUBSTITUTE(G34," ","_"))/1000000,(E34-F34)*J34))</f>
         <v/>
       </c>
@@ -2503,7 +2497,7 @@
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
-      <c r="K35" s="15" t="str">
+      <c r="K35" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E35),AND(OR(ISBLANK(G35),ISBLANK(H35),ISBLANK(I35)),ISBLANK(J35))),"",IF(ISBLANK(J35),(E35-F35)*I35*H35*INDIRECT(SUBSTITUTE(G35," ","_"))/1000000,(E35-F35)*J35))</f>
         <v/>
       </c>
@@ -2526,7 +2520,7 @@
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
-      <c r="K36" s="15" t="str">
+      <c r="K36" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E36),AND(OR(ISBLANK(G36),ISBLANK(H36),ISBLANK(I36)),ISBLANK(J36))),"",IF(ISBLANK(J36),(E36-F36)*I36*H36*INDIRECT(SUBSTITUTE(G36," ","_"))/1000000,(E36-F36)*J36))</f>
         <v/>
       </c>
@@ -2549,7 +2543,7 @@
       <c r="H37" s="15"/>
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
-      <c r="K37" s="15" t="str">
+      <c r="K37" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E37),AND(OR(ISBLANK(G37),ISBLANK(H37),ISBLANK(I37)),ISBLANK(J37))),"",IF(ISBLANK(J37),(E37-F37)*I37*H37*INDIRECT(SUBSTITUTE(G37," ","_"))/1000000,(E37-F37)*J37))</f>
         <v/>
       </c>
@@ -2572,7 +2566,7 @@
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
       <c r="J38" s="15"/>
-      <c r="K38" s="15" t="str">
+      <c r="K38" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E38),AND(OR(ISBLANK(G38),ISBLANK(H38),ISBLANK(I38)),ISBLANK(J38))),"",IF(ISBLANK(J38),(E38-F38)*I38*H38*INDIRECT(SUBSTITUTE(G38," ","_"))/1000000,(E38-F38)*J38))</f>
         <v/>
       </c>
@@ -2595,7 +2589,7 @@
       <c r="H39" s="15"/>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
-      <c r="K39" s="15" t="str">
+      <c r="K39" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E39),AND(OR(ISBLANK(G39),ISBLANK(H39),ISBLANK(I39)),ISBLANK(J39))),"",IF(ISBLANK(J39),(E39-F39)*I39*H39*INDIRECT(SUBSTITUTE(G39," ","_"))/1000000,(E39-F39)*J39))</f>
         <v/>
       </c>
@@ -2618,7 +2612,7 @@
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
-      <c r="K40" s="15" t="str">
+      <c r="K40" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E40),AND(OR(ISBLANK(G40),ISBLANK(H40),ISBLANK(I40)),ISBLANK(J40))),"",IF(ISBLANK(J40),(E40-F40)*I40*H40*INDIRECT(SUBSTITUTE(G40," ","_"))/1000000,(E40-F40)*J40))</f>
         <v/>
       </c>
@@ -2641,7 +2635,7 @@
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
-      <c r="K41" s="15" t="str">
+      <c r="K41" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E41),AND(OR(ISBLANK(G41),ISBLANK(H41),ISBLANK(I41)),ISBLANK(J41))),"",IF(ISBLANK(J41),(E41-F41)*I41*H41*INDIRECT(SUBSTITUTE(G41," ","_"))/1000000,(E41-F41)*J41))</f>
         <v/>
       </c>
@@ -2664,7 +2658,7 @@
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
-      <c r="K42" s="15" t="str">
+      <c r="K42" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E42),AND(OR(ISBLANK(G42),ISBLANK(H42),ISBLANK(I42)),ISBLANK(J42))),"",IF(ISBLANK(J42),(E42-F42)*I42*H42*INDIRECT(SUBSTITUTE(G42," ","_"))/1000000,(E42-F42)*J42))</f>
         <v/>
       </c>
@@ -2687,7 +2681,7 @@
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
-      <c r="K43" s="15" t="str">
+      <c r="K43" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E43),AND(OR(ISBLANK(G43),ISBLANK(H43),ISBLANK(I43)),ISBLANK(J43))),"",IF(ISBLANK(J43),(E43-F43)*I43*H43*INDIRECT(SUBSTITUTE(G43," ","_"))/1000000,(E43-F43)*J43))</f>
         <v/>
       </c>
@@ -2710,7 +2704,7 @@
       <c r="H44" s="15"/>
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
-      <c r="K44" s="15" t="str">
+      <c r="K44" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E44),AND(OR(ISBLANK(G44),ISBLANK(H44),ISBLANK(I44)),ISBLANK(J44))),"",IF(ISBLANK(J44),(E44-F44)*I44*H44*INDIRECT(SUBSTITUTE(G44," ","_"))/1000000,(E44-F44)*J44))</f>
         <v/>
       </c>
@@ -2733,7 +2727,7 @@
       <c r="H45" s="15"/>
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
-      <c r="K45" s="15" t="str">
+      <c r="K45" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E45),AND(OR(ISBLANK(G45),ISBLANK(H45),ISBLANK(I45)),ISBLANK(J45))),"",IF(ISBLANK(J45),(E45-F45)*I45*H45*INDIRECT(SUBSTITUTE(G45," ","_"))/1000000,(E45-F45)*J45))</f>
         <v/>
       </c>
@@ -2756,7 +2750,7 @@
       <c r="H46" s="15"/>
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
-      <c r="K46" s="15" t="str">
+      <c r="K46" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E46),AND(OR(ISBLANK(G46),ISBLANK(H46),ISBLANK(I46)),ISBLANK(J46))),"",IF(ISBLANK(J46),(E46-F46)*I46*H46*INDIRECT(SUBSTITUTE(G46," ","_"))/1000000,(E46-F46)*J46))</f>
         <v/>
       </c>
@@ -2779,7 +2773,7 @@
       <c r="H47" s="15"/>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
-      <c r="K47" s="15" t="str">
+      <c r="K47" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E47),AND(OR(ISBLANK(G47),ISBLANK(H47),ISBLANK(I47)),ISBLANK(J47))),"",IF(ISBLANK(J47),(E47-F47)*I47*H47*INDIRECT(SUBSTITUTE(G47," ","_"))/1000000,(E47-F47)*J47))</f>
         <v/>
       </c>
@@ -2802,7 +2796,7 @@
       <c r="H48" s="15"/>
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
-      <c r="K48" s="15" t="str">
+      <c r="K48" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E48),AND(OR(ISBLANK(G48),ISBLANK(H48),ISBLANK(I48)),ISBLANK(J48))),"",IF(ISBLANK(J48),(E48-F48)*I48*H48*INDIRECT(SUBSTITUTE(G48," ","_"))/1000000,(E48-F48)*J48))</f>
         <v/>
       </c>
@@ -2825,7 +2819,7 @@
       <c r="H49" s="15"/>
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
-      <c r="K49" s="15" t="str">
+      <c r="K49" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E49),AND(OR(ISBLANK(G49),ISBLANK(H49),ISBLANK(I49)),ISBLANK(J49))),"",IF(ISBLANK(J49),(E49-F49)*I49*H49*INDIRECT(SUBSTITUTE(G49," ","_"))/1000000,(E49-F49)*J49))</f>
         <v/>
       </c>
@@ -2848,7 +2842,7 @@
       <c r="H50" s="15"/>
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
-      <c r="K50" s="15" t="str">
+      <c r="K50" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E50),AND(OR(ISBLANK(G50),ISBLANK(H50),ISBLANK(I50)),ISBLANK(J50))),"",IF(ISBLANK(J50),(E50-F50)*I50*H50*INDIRECT(SUBSTITUTE(G50," ","_"))/1000000,(E50-F50)*J50))</f>
         <v/>
       </c>
@@ -2871,7 +2865,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
-      <c r="K51" s="15" t="str">
+      <c r="K51" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E51),AND(OR(ISBLANK(G51),ISBLANK(H51),ISBLANK(I51)),ISBLANK(J51))),"",IF(ISBLANK(J51),(E51-F51)*I51*H51*INDIRECT(SUBSTITUTE(G51," ","_"))/1000000,(E51-F51)*J51))</f>
         <v/>
       </c>
@@ -2894,7 +2888,7 @@
       <c r="H52" s="15"/>
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
-      <c r="K52" s="15" t="str">
+      <c r="K52" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E52),AND(OR(ISBLANK(G52),ISBLANK(H52),ISBLANK(I52)),ISBLANK(J52))),"",IF(ISBLANK(J52),(E52-F52)*I52*H52*INDIRECT(SUBSTITUTE(G52," ","_"))/1000000,(E52-F52)*J52))</f>
         <v/>
       </c>
@@ -2917,7 +2911,7 @@
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
-      <c r="K53" s="15" t="str">
+      <c r="K53" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E53),AND(OR(ISBLANK(G53),ISBLANK(H53),ISBLANK(I53)),ISBLANK(J53))),"",IF(ISBLANK(J53),(E53-F53)*I53*H53*INDIRECT(SUBSTITUTE(G53," ","_"))/1000000,(E53-F53)*J53))</f>
         <v/>
       </c>
@@ -2940,7 +2934,7 @@
       <c r="H54" s="15"/>
       <c r="I54" s="15"/>
       <c r="J54" s="15"/>
-      <c r="K54" s="15" t="str">
+      <c r="K54" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E54),AND(OR(ISBLANK(G54),ISBLANK(H54),ISBLANK(I54)),ISBLANK(J54))),"",IF(ISBLANK(J54),(E54-F54)*I54*H54*INDIRECT(SUBSTITUTE(G54," ","_"))/1000000,(E54-F54)*J54))</f>
         <v/>
       </c>
@@ -2963,7 +2957,7 @@
       <c r="H55" s="15"/>
       <c r="I55" s="15"/>
       <c r="J55" s="15"/>
-      <c r="K55" s="15" t="str">
+      <c r="K55" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E55),AND(OR(ISBLANK(G55),ISBLANK(H55),ISBLANK(I55)),ISBLANK(J55))),"",IF(ISBLANK(J55),(E55-F55)*I55*H55*INDIRECT(SUBSTITUTE(G55," ","_"))/1000000,(E55-F55)*J55))</f>
         <v/>
       </c>
@@ -2986,7 +2980,7 @@
       <c r="H56" s="15"/>
       <c r="I56" s="15"/>
       <c r="J56" s="15"/>
-      <c r="K56" s="15" t="str">
+      <c r="K56" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E56),AND(OR(ISBLANK(G56),ISBLANK(H56),ISBLANK(I56)),ISBLANK(J56))),"",IF(ISBLANK(J56),(E56-F56)*I56*H56*INDIRECT(SUBSTITUTE(G56," ","_"))/1000000,(E56-F56)*J56))</f>
         <v/>
       </c>
@@ -3009,7 +3003,7 @@
       <c r="H57" s="15"/>
       <c r="I57" s="15"/>
       <c r="J57" s="15"/>
-      <c r="K57" s="15" t="str">
+      <c r="K57" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E57),AND(OR(ISBLANK(G57),ISBLANK(H57),ISBLANK(I57)),ISBLANK(J57))),"",IF(ISBLANK(J57),(E57-F57)*I57*H57*INDIRECT(SUBSTITUTE(G57," ","_"))/1000000,(E57-F57)*J57))</f>
         <v/>
       </c>
@@ -3032,7 +3026,7 @@
       <c r="H58" s="15"/>
       <c r="I58" s="15"/>
       <c r="J58" s="15"/>
-      <c r="K58" s="15" t="str">
+      <c r="K58" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E58),AND(OR(ISBLANK(G58),ISBLANK(H58),ISBLANK(I58)),ISBLANK(J58))),"",IF(ISBLANK(J58),(E58-F58)*I58*H58*INDIRECT(SUBSTITUTE(G58," ","_"))/1000000,(E58-F58)*J58))</f>
         <v/>
       </c>
@@ -3055,7 +3049,7 @@
       <c r="H59" s="15"/>
       <c r="I59" s="15"/>
       <c r="J59" s="15"/>
-      <c r="K59" s="15" t="str">
+      <c r="K59" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E59),AND(OR(ISBLANK(G59),ISBLANK(H59),ISBLANK(I59)),ISBLANK(J59))),"",IF(ISBLANK(J59),(E59-F59)*I59*H59*INDIRECT(SUBSTITUTE(G59," ","_"))/1000000,(E59-F59)*J59))</f>
         <v/>
       </c>
@@ -3078,7 +3072,7 @@
       <c r="H60" s="15"/>
       <c r="I60" s="15"/>
       <c r="J60" s="15"/>
-      <c r="K60" s="15" t="str">
+      <c r="K60" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E60),AND(OR(ISBLANK(G60),ISBLANK(H60),ISBLANK(I60)),ISBLANK(J60))),"",IF(ISBLANK(J60),(E60-F60)*I60*H60*INDIRECT(SUBSTITUTE(G60," ","_"))/1000000,(E60-F60)*J60))</f>
         <v/>
       </c>
@@ -3101,7 +3095,7 @@
       <c r="H61" s="15"/>
       <c r="I61" s="15"/>
       <c r="J61" s="15"/>
-      <c r="K61" s="15" t="str">
+      <c r="K61" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E61),AND(OR(ISBLANK(G61),ISBLANK(H61),ISBLANK(I61)),ISBLANK(J61))),"",IF(ISBLANK(J61),(E61-F61)*I61*H61*INDIRECT(SUBSTITUTE(G61," ","_"))/1000000,(E61-F61)*J61))</f>
         <v/>
       </c>
@@ -3124,7 +3118,7 @@
       <c r="H62" s="15"/>
       <c r="I62" s="15"/>
       <c r="J62" s="15"/>
-      <c r="K62" s="15" t="str">
+      <c r="K62" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E62),AND(OR(ISBLANK(G62),ISBLANK(H62),ISBLANK(I62)),ISBLANK(J62))),"",IF(ISBLANK(J62),(E62-F62)*I62*H62*INDIRECT(SUBSTITUTE(G62," ","_"))/1000000,(E62-F62)*J62))</f>
         <v/>
       </c>
@@ -3147,7 +3141,7 @@
       <c r="H63" s="15"/>
       <c r="I63" s="15"/>
       <c r="J63" s="15"/>
-      <c r="K63" s="15" t="str">
+      <c r="K63" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E63),AND(OR(ISBLANK(G63),ISBLANK(H63),ISBLANK(I63)),ISBLANK(J63))),"",IF(ISBLANK(J63),(E63-F63)*I63*H63*INDIRECT(SUBSTITUTE(G63," ","_"))/1000000,(E63-F63)*J63))</f>
         <v/>
       </c>
@@ -3170,7 +3164,7 @@
       <c r="H64" s="15"/>
       <c r="I64" s="15"/>
       <c r="J64" s="15"/>
-      <c r="K64" s="15" t="str">
+      <c r="K64" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E64),AND(OR(ISBLANK(G64),ISBLANK(H64),ISBLANK(I64)),ISBLANK(J64))),"",IF(ISBLANK(J64),(E64-F64)*I64*H64*INDIRECT(SUBSTITUTE(G64," ","_"))/1000000,(E64-F64)*J64))</f>
         <v/>
       </c>
@@ -3193,7 +3187,7 @@
       <c r="H65" s="15"/>
       <c r="I65" s="15"/>
       <c r="J65" s="15"/>
-      <c r="K65" s="15" t="str">
+      <c r="K65" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E65),AND(OR(ISBLANK(G65),ISBLANK(H65),ISBLANK(I65)),ISBLANK(J65))),"",IF(ISBLANK(J65),(E65-F65)*I65*H65*INDIRECT(SUBSTITUTE(G65," ","_"))/1000000,(E65-F65)*J65))</f>
         <v/>
       </c>
@@ -3216,7 +3210,7 @@
       <c r="H66" s="15"/>
       <c r="I66" s="15"/>
       <c r="J66" s="15"/>
-      <c r="K66" s="15" t="str">
+      <c r="K66" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E66),AND(OR(ISBLANK(G66),ISBLANK(H66),ISBLANK(I66)),ISBLANK(J66))),"",IF(ISBLANK(J66),(E66-F66)*I66*H66*INDIRECT(SUBSTITUTE(G66," ","_"))/1000000,(E66-F66)*J66))</f>
         <v/>
       </c>
@@ -3239,7 +3233,7 @@
       <c r="H67" s="15"/>
       <c r="I67" s="15"/>
       <c r="J67" s="15"/>
-      <c r="K67" s="15" t="str">
+      <c r="K67" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E67),AND(OR(ISBLANK(G67),ISBLANK(H67),ISBLANK(I67)),ISBLANK(J67))),"",IF(ISBLANK(J67),(E67-F67)*I67*H67*INDIRECT(SUBSTITUTE(G67," ","_"))/1000000,(E67-F67)*J67))</f>
         <v/>
       </c>
@@ -3262,7 +3256,7 @@
       <c r="H68" s="15"/>
       <c r="I68" s="15"/>
       <c r="J68" s="15"/>
-      <c r="K68" s="15" t="str">
+      <c r="K68" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E68),AND(OR(ISBLANK(G68),ISBLANK(H68),ISBLANK(I68)),ISBLANK(J68))),"",IF(ISBLANK(J68),(E68-F68)*I68*H68*INDIRECT(SUBSTITUTE(G68," ","_"))/1000000,(E68-F68)*J68))</f>
         <v/>
       </c>
@@ -3285,7 +3279,7 @@
       <c r="H69" s="15"/>
       <c r="I69" s="15"/>
       <c r="J69" s="15"/>
-      <c r="K69" s="15" t="str">
+      <c r="K69" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E69),AND(OR(ISBLANK(G69),ISBLANK(H69),ISBLANK(I69)),ISBLANK(J69))),"",IF(ISBLANK(J69),(E69-F69)*I69*H69*INDIRECT(SUBSTITUTE(G69," ","_"))/1000000,(E69-F69)*J69))</f>
         <v/>
       </c>
@@ -3308,7 +3302,7 @@
       <c r="H70" s="15"/>
       <c r="I70" s="15"/>
       <c r="J70" s="15"/>
-      <c r="K70" s="15" t="str">
+      <c r="K70" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E70),AND(OR(ISBLANK(G70),ISBLANK(H70),ISBLANK(I70)),ISBLANK(J70))),"",IF(ISBLANK(J70),(E70-F70)*I70*H70*INDIRECT(SUBSTITUTE(G70," ","_"))/1000000,(E70-F70)*J70))</f>
         <v/>
       </c>
@@ -3331,7 +3325,7 @@
       <c r="H71" s="15"/>
       <c r="I71" s="15"/>
       <c r="J71" s="15"/>
-      <c r="K71" s="15" t="str">
+      <c r="K71" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E71),AND(OR(ISBLANK(G71),ISBLANK(H71),ISBLANK(I71)),ISBLANK(J71))),"",IF(ISBLANK(J71),(E71-F71)*I71*H71*INDIRECT(SUBSTITUTE(G71," ","_"))/1000000,(E71-F71)*J71))</f>
         <v/>
       </c>
@@ -3354,7 +3348,7 @@
       <c r="H72" s="15"/>
       <c r="I72" s="15"/>
       <c r="J72" s="15"/>
-      <c r="K72" s="15" t="str">
+      <c r="K72" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E72),AND(OR(ISBLANK(G72),ISBLANK(H72),ISBLANK(I72)),ISBLANK(J72))),"",IF(ISBLANK(J72),(E72-F72)*I72*H72*INDIRECT(SUBSTITUTE(G72," ","_"))/1000000,(E72-F72)*J72))</f>
         <v/>
       </c>
@@ -3377,7 +3371,7 @@
       <c r="H73" s="15"/>
       <c r="I73" s="15"/>
       <c r="J73" s="15"/>
-      <c r="K73" s="15" t="str">
+      <c r="K73" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E73),AND(OR(ISBLANK(G73),ISBLANK(H73),ISBLANK(I73)),ISBLANK(J73))),"",IF(ISBLANK(J73),(E73-F73)*I73*H73*INDIRECT(SUBSTITUTE(G73," ","_"))/1000000,(E73-F73)*J73))</f>
         <v/>
       </c>
@@ -3400,7 +3394,7 @@
       <c r="H74" s="15"/>
       <c r="I74" s="15"/>
       <c r="J74" s="15"/>
-      <c r="K74" s="15" t="str">
+      <c r="K74" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E74),AND(OR(ISBLANK(G74),ISBLANK(H74),ISBLANK(I74)),ISBLANK(J74))),"",IF(ISBLANK(J74),(E74-F74)*I74*H74*INDIRECT(SUBSTITUTE(G74," ","_"))/1000000,(E74-F74)*J74))</f>
         <v/>
       </c>
@@ -3423,7 +3417,7 @@
       <c r="H75" s="15"/>
       <c r="I75" s="15"/>
       <c r="J75" s="15"/>
-      <c r="K75" s="15" t="str">
+      <c r="K75" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E75),AND(OR(ISBLANK(G75),ISBLANK(H75),ISBLANK(I75)),ISBLANK(J75))),"",IF(ISBLANK(J75),(E75-F75)*I75*H75*INDIRECT(SUBSTITUTE(G75," ","_"))/1000000,(E75-F75)*J75))</f>
         <v/>
       </c>
@@ -3446,7 +3440,7 @@
       <c r="H76" s="15"/>
       <c r="I76" s="15"/>
       <c r="J76" s="15"/>
-      <c r="K76" s="15" t="str">
+      <c r="K76" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E76),AND(OR(ISBLANK(G76),ISBLANK(H76),ISBLANK(I76)),ISBLANK(J76))),"",IF(ISBLANK(J76),(E76-F76)*I76*H76*INDIRECT(SUBSTITUTE(G76," ","_"))/1000000,(E76-F76)*J76))</f>
         <v/>
       </c>
@@ -3469,7 +3463,7 @@
       <c r="H77" s="15"/>
       <c r="I77" s="15"/>
       <c r="J77" s="15"/>
-      <c r="K77" s="15" t="str">
+      <c r="K77" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E77),AND(OR(ISBLANK(G77),ISBLANK(H77),ISBLANK(I77)),ISBLANK(J77))),"",IF(ISBLANK(J77),(E77-F77)*I77*H77*INDIRECT(SUBSTITUTE(G77," ","_"))/1000000,(E77-F77)*J77))</f>
         <v/>
       </c>
@@ -3492,7 +3486,7 @@
       <c r="H78" s="15"/>
       <c r="I78" s="15"/>
       <c r="J78" s="15"/>
-      <c r="K78" s="15" t="str">
+      <c r="K78" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E78),AND(OR(ISBLANK(G78),ISBLANK(H78),ISBLANK(I78)),ISBLANK(J78))),"",IF(ISBLANK(J78),(E78-F78)*I78*H78*INDIRECT(SUBSTITUTE(G78," ","_"))/1000000,(E78-F78)*J78))</f>
         <v/>
       </c>
@@ -3515,7 +3509,7 @@
       <c r="H79" s="15"/>
       <c r="I79" s="15"/>
       <c r="J79" s="15"/>
-      <c r="K79" s="15" t="str">
+      <c r="K79" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E79),AND(OR(ISBLANK(G79),ISBLANK(H79),ISBLANK(I79)),ISBLANK(J79))),"",IF(ISBLANK(J79),(E79-F79)*I79*H79*INDIRECT(SUBSTITUTE(G79," ","_"))/1000000,(E79-F79)*J79))</f>
         <v/>
       </c>
@@ -3538,7 +3532,7 @@
       <c r="H80" s="15"/>
       <c r="I80" s="15"/>
       <c r="J80" s="15"/>
-      <c r="K80" s="15" t="str">
+      <c r="K80" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E80),AND(OR(ISBLANK(G80),ISBLANK(H80),ISBLANK(I80)),ISBLANK(J80))),"",IF(ISBLANK(J80),(E80-F80)*I80*H80*INDIRECT(SUBSTITUTE(G80," ","_"))/1000000,(E80-F80)*J80))</f>
         <v/>
       </c>
@@ -3561,7 +3555,7 @@
       <c r="H81" s="15"/>
       <c r="I81" s="15"/>
       <c r="J81" s="15"/>
-      <c r="K81" s="15" t="str">
+      <c r="K81" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E81),AND(OR(ISBLANK(G81),ISBLANK(H81),ISBLANK(I81)),ISBLANK(J81))),"",IF(ISBLANK(J81),(E81-F81)*I81*H81*INDIRECT(SUBSTITUTE(G81," ","_"))/1000000,(E81-F81)*J81))</f>
         <v/>
       </c>
@@ -3584,7 +3578,7 @@
       <c r="H82" s="15"/>
       <c r="I82" s="15"/>
       <c r="J82" s="15"/>
-      <c r="K82" s="15" t="str">
+      <c r="K82" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E82),AND(OR(ISBLANK(G82),ISBLANK(H82),ISBLANK(I82)),ISBLANK(J82))),"",IF(ISBLANK(J82),(E82-F82)*I82*H82*INDIRECT(SUBSTITUTE(G82," ","_"))/1000000,(E82-F82)*J82))</f>
         <v/>
       </c>
@@ -3607,7 +3601,7 @@
       <c r="H83" s="15"/>
       <c r="I83" s="15"/>
       <c r="J83" s="15"/>
-      <c r="K83" s="15" t="str">
+      <c r="K83" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E83),AND(OR(ISBLANK(G83),ISBLANK(H83),ISBLANK(I83)),ISBLANK(J83))),"",IF(ISBLANK(J83),(E83-F83)*I83*H83*INDIRECT(SUBSTITUTE(G83," ","_"))/1000000,(E83-F83)*J83))</f>
         <v/>
       </c>
@@ -3630,7 +3624,7 @@
       <c r="H84" s="15"/>
       <c r="I84" s="15"/>
       <c r="J84" s="15"/>
-      <c r="K84" s="15" t="str">
+      <c r="K84" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E84),AND(OR(ISBLANK(G84),ISBLANK(H84),ISBLANK(I84)),ISBLANK(J84))),"",IF(ISBLANK(J84),(E84-F84)*I84*H84*INDIRECT(SUBSTITUTE(G84," ","_"))/1000000,(E84-F84)*J84))</f>
         <v/>
       </c>
@@ -3653,7 +3647,7 @@
       <c r="H85" s="15"/>
       <c r="I85" s="15"/>
       <c r="J85" s="15"/>
-      <c r="K85" s="15" t="str">
+      <c r="K85" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E85),AND(OR(ISBLANK(G85),ISBLANK(H85),ISBLANK(I85)),ISBLANK(J85))),"",IF(ISBLANK(J85),(E85-F85)*I85*H85*INDIRECT(SUBSTITUTE(G85," ","_"))/1000000,(E85-F85)*J85))</f>
         <v/>
       </c>
@@ -3676,7 +3670,7 @@
       <c r="H86" s="15"/>
       <c r="I86" s="15"/>
       <c r="J86" s="15"/>
-      <c r="K86" s="15" t="str">
+      <c r="K86" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E86),AND(OR(ISBLANK(G86),ISBLANK(H86),ISBLANK(I86)),ISBLANK(J86))),"",IF(ISBLANK(J86),(E86-F86)*I86*H86*INDIRECT(SUBSTITUTE(G86," ","_"))/1000000,(E86-F86)*J86))</f>
         <v/>
       </c>
@@ -3699,7 +3693,7 @@
       <c r="H87" s="15"/>
       <c r="I87" s="15"/>
       <c r="J87" s="15"/>
-      <c r="K87" s="15" t="str">
+      <c r="K87" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E87),AND(OR(ISBLANK(G87),ISBLANK(H87),ISBLANK(I87)),ISBLANK(J87))),"",IF(ISBLANK(J87),(E87-F87)*I87*H87*INDIRECT(SUBSTITUTE(G87," ","_"))/1000000,(E87-F87)*J87))</f>
         <v/>
       </c>
@@ -3722,7 +3716,7 @@
       <c r="H88" s="15"/>
       <c r="I88" s="15"/>
       <c r="J88" s="15"/>
-      <c r="K88" s="15" t="str">
+      <c r="K88" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E88),AND(OR(ISBLANK(G88),ISBLANK(H88),ISBLANK(I88)),ISBLANK(J88))),"",IF(ISBLANK(J88),(E88-F88)*I88*H88*INDIRECT(SUBSTITUTE(G88," ","_"))/1000000,(E88-F88)*J88))</f>
         <v/>
       </c>
@@ -3745,7 +3739,7 @@
       <c r="H89" s="15"/>
       <c r="I89" s="15"/>
       <c r="J89" s="15"/>
-      <c r="K89" s="15" t="str">
+      <c r="K89" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E89),AND(OR(ISBLANK(G89),ISBLANK(H89),ISBLANK(I89)),ISBLANK(J89))),"",IF(ISBLANK(J89),(E89-F89)*I89*H89*INDIRECT(SUBSTITUTE(G89," ","_"))/1000000,(E89-F89)*J89))</f>
         <v/>
       </c>
@@ -3768,7 +3762,7 @@
       <c r="H90" s="15"/>
       <c r="I90" s="15"/>
       <c r="J90" s="15"/>
-      <c r="K90" s="15" t="str">
+      <c r="K90" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E90),AND(OR(ISBLANK(G90),ISBLANK(H90),ISBLANK(I90)),ISBLANK(J90))),"",IF(ISBLANK(J90),(E90-F90)*I90*H90*INDIRECT(SUBSTITUTE(G90," ","_"))/1000000,(E90-F90)*J90))</f>
         <v/>
       </c>
@@ -3791,7 +3785,7 @@
       <c r="H91" s="15"/>
       <c r="I91" s="15"/>
       <c r="J91" s="15"/>
-      <c r="K91" s="15" t="str">
+      <c r="K91" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E91),AND(OR(ISBLANK(G91),ISBLANK(H91),ISBLANK(I91)),ISBLANK(J91))),"",IF(ISBLANK(J91),(E91-F91)*I91*H91*INDIRECT(SUBSTITUTE(G91," ","_"))/1000000,(E91-F91)*J91))</f>
         <v/>
       </c>
@@ -3814,7 +3808,7 @@
       <c r="H92" s="15"/>
       <c r="I92" s="15"/>
       <c r="J92" s="15"/>
-      <c r="K92" s="15" t="str">
+      <c r="K92" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E92),AND(OR(ISBLANK(G92),ISBLANK(H92),ISBLANK(I92)),ISBLANK(J92))),"",IF(ISBLANK(J92),(E92-F92)*I92*H92*INDIRECT(SUBSTITUTE(G92," ","_"))/1000000,(E92-F92)*J92))</f>
         <v/>
       </c>
@@ -3837,7 +3831,7 @@
       <c r="H93" s="15"/>
       <c r="I93" s="15"/>
       <c r="J93" s="15"/>
-      <c r="K93" s="15" t="str">
+      <c r="K93" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E93),AND(OR(ISBLANK(G93),ISBLANK(H93),ISBLANK(I93)),ISBLANK(J93))),"",IF(ISBLANK(J93),(E93-F93)*I93*H93*INDIRECT(SUBSTITUTE(G93," ","_"))/1000000,(E93-F93)*J93))</f>
         <v/>
       </c>
@@ -3860,7 +3854,7 @@
       <c r="H94" s="15"/>
       <c r="I94" s="15"/>
       <c r="J94" s="15"/>
-      <c r="K94" s="15" t="str">
+      <c r="K94" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E94),AND(OR(ISBLANK(G94),ISBLANK(H94),ISBLANK(I94)),ISBLANK(J94))),"",IF(ISBLANK(J94),(E94-F94)*I94*H94*INDIRECT(SUBSTITUTE(G94," ","_"))/1000000,(E94-F94)*J94))</f>
         <v/>
       </c>
@@ -3883,7 +3877,7 @@
       <c r="H95" s="15"/>
       <c r="I95" s="15"/>
       <c r="J95" s="15"/>
-      <c r="K95" s="15" t="str">
+      <c r="K95" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E95),AND(OR(ISBLANK(G95),ISBLANK(H95),ISBLANK(I95)),ISBLANK(J95))),"",IF(ISBLANK(J95),(E95-F95)*I95*H95*INDIRECT(SUBSTITUTE(G95," ","_"))/1000000,(E95-F95)*J95))</f>
         <v/>
       </c>
@@ -3906,7 +3900,7 @@
       <c r="H96" s="15"/>
       <c r="I96" s="15"/>
       <c r="J96" s="15"/>
-      <c r="K96" s="15" t="str">
+      <c r="K96" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E96),AND(OR(ISBLANK(G96),ISBLANK(H96),ISBLANK(I96)),ISBLANK(J96))),"",IF(ISBLANK(J96),(E96-F96)*I96*H96*INDIRECT(SUBSTITUTE(G96," ","_"))/1000000,(E96-F96)*J96))</f>
         <v/>
       </c>
@@ -3929,7 +3923,7 @@
       <c r="H97" s="15"/>
       <c r="I97" s="15"/>
       <c r="J97" s="15"/>
-      <c r="K97" s="15" t="str">
+      <c r="K97" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E97),AND(OR(ISBLANK(G97),ISBLANK(H97),ISBLANK(I97)),ISBLANK(J97))),"",IF(ISBLANK(J97),(E97-F97)*I97*H97*INDIRECT(SUBSTITUTE(G97," ","_"))/1000000,(E97-F97)*J97))</f>
         <v/>
       </c>
@@ -3952,7 +3946,7 @@
       <c r="H98" s="15"/>
       <c r="I98" s="15"/>
       <c r="J98" s="15"/>
-      <c r="K98" s="15" t="str">
+      <c r="K98" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E98),AND(OR(ISBLANK(G98),ISBLANK(H98),ISBLANK(I98)),ISBLANK(J98))),"",IF(ISBLANK(J98),(E98-F98)*I98*H98*INDIRECT(SUBSTITUTE(G98," ","_"))/1000000,(E98-F98)*J98))</f>
         <v/>
       </c>
@@ -3975,7 +3969,7 @@
       <c r="H99" s="15"/>
       <c r="I99" s="15"/>
       <c r="J99" s="15"/>
-      <c r="K99" s="15" t="str">
+      <c r="K99" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E99),AND(OR(ISBLANK(G99),ISBLANK(H99),ISBLANK(I99)),ISBLANK(J99))),"",IF(ISBLANK(J99),(E99-F99)*I99*H99*INDIRECT(SUBSTITUTE(G99," ","_"))/1000000,(E99-F99)*J99))</f>
         <v/>
       </c>
@@ -3998,7 +3992,7 @@
       <c r="H100" s="15"/>
       <c r="I100" s="15"/>
       <c r="J100" s="15"/>
-      <c r="K100" s="15" t="str">
+      <c r="K100" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E100),AND(OR(ISBLANK(G100),ISBLANK(H100),ISBLANK(I100)),ISBLANK(J100))),"",IF(ISBLANK(J100),(E100-F100)*I100*H100*INDIRECT(SUBSTITUTE(G100," ","_"))/1000000,(E100-F100)*J100))</f>
         <v/>
       </c>
@@ -4021,7 +4015,7 @@
       <c r="H101" s="15"/>
       <c r="I101" s="15"/>
       <c r="J101" s="15"/>
-      <c r="K101" s="15" t="str">
+      <c r="K101" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E101),AND(OR(ISBLANK(G101),ISBLANK(H101),ISBLANK(I101)),ISBLANK(J101))),"",IF(ISBLANK(J101),(E101-F101)*I101*H101*INDIRECT(SUBSTITUTE(G101," ","_"))/1000000,(E101-F101)*J101))</f>
         <v/>
       </c>
@@ -4044,7 +4038,7 @@
       <c r="H102" s="15"/>
       <c r="I102" s="15"/>
       <c r="J102" s="15"/>
-      <c r="K102" s="15" t="str">
+      <c r="K102" s="12" t="str">
         <f aca="true">IF(OR(ISBLANK(E102),AND(OR(ISBLANK(G102),ISBLANK(H102),ISBLANK(I102)),ISBLANK(J102))),"",IF(ISBLANK(J102),(E102-F102)*I102*H102*INDIRECT(SUBSTITUTE(G102," ","_"))/1000000,(E102-F102)*J102))</f>
         <v/>
       </c>
@@ -4067,7 +4061,7 @@
       <c r="H103" s="25"/>
       <c r="I103" s="25"/>
       <c r="J103" s="25"/>
-      <c r="K103" s="25" t="str">
+      <c r="K103" s="26" t="str">
         <f aca="true">IF(OR(ISBLANK(E103),AND(OR(ISBLANK(G103),ISBLANK(H103),ISBLANK(I103)),ISBLANK(J103))),"",IF(ISBLANK(J103),(E103-F103)*I103*H103*INDIRECT(SUBSTITUTE(G103," ","_"))/1000000,(E103-F103)*J103))</f>
         <v/>
       </c>
@@ -4075,9 +4069,9 @@
       <c r="M103" s="25"/>
       <c r="N103" s="24"/>
       <c r="O103" s="21"/>
-      <c r="P103" s="26"/>
-      <c r="Q103" s="27"/>
-      <c r="R103" s="28"/>
+      <c r="P103" s="27"/>
+      <c r="Q103" s="28"/>
+      <c r="R103" s="29"/>
     </row>
     <row r="104" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O104" s="3"/>
@@ -6815,7 +6809,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.5"/>
@@ -6828,2357 +6822,2357 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29" t="s">
+      <c r="J1" s="30"/>
+      <c r="K1" s="30" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="30" t="n">
+      <c r="G2" s="30"/>
+      <c r="H2" s="31" t="n">
         <v>607.558</v>
       </c>
-      <c r="I2" s="30" t="n">
+      <c r="I2" s="31" t="n">
         <v>303.779</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29" t="s">
+      <c r="J2" s="30"/>
+      <c r="K2" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29" t="s">
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29" t="s">
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="31" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="E9" s="31" t="s">
+      <c r="C9" s="30"/>
+      <c r="E9" s="30" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="29"/>
+      <c r="C10" s="30"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="29"/>
+      <c r="C11" s="30"/>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="29"/>
+      <c r="C12" s="30"/>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="29"/>
+      <c r="C13" s="30"/>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="29"/>
+      <c r="C14" s="30"/>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="30" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="30" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="30" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="30" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="30" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="30" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="30" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="30" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="30" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="30" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="30" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="30" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="30" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="30" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="30" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="30" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="30" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="30" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="30" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="30" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="30" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="30" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="30" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B41" s="29" t="s">
+      <c r="B41" s="30" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="30" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="30" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="30" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="30" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="30" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="30" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="30" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="B49" s="29" t="s">
+      <c r="B49" s="30" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="B50" s="29" t="s">
+      <c r="B50" s="30" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="30" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="B52" s="29" t="s">
+      <c r="B52" s="30" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="30" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="29" t="s">
+      <c r="A54" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="30" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="30" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="B56" s="29" t="s">
+      <c r="B56" s="30" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="29" t="s">
+      <c r="A57" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="B57" s="29" t="s">
+      <c r="B57" s="30" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="29" t="s">
+      <c r="A58" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="30" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="29" t="s">
+      <c r="A59" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="29" t="s">
+      <c r="B59" s="30" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="29" t="s">
+      <c r="A60" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="29" t="s">
+      <c r="B60" s="30" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="29" t="s">
+      <c r="A61" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="B61" s="29" t="s">
+      <c r="B61" s="30" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="29" t="s">
+      <c r="A62" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="B62" s="29" t="s">
+      <c r="B62" s="30" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="29" t="s">
+      <c r="A63" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="B63" s="29" t="s">
+      <c r="B63" s="30" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="29" t="s">
+      <c r="A64" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B64" s="29" t="s">
+      <c r="B64" s="30" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="29" t="s">
+      <c r="A65" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="B65" s="29" t="s">
+      <c r="B65" s="30" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="29" t="s">
+      <c r="A66" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="B66" s="29" t="s">
+      <c r="B66" s="30" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="29" t="s">
+      <c r="A67" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="B67" s="29" t="s">
+      <c r="B67" s="30" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="29" t="s">
+      <c r="A68" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="B68" s="29" t="s">
+      <c r="B68" s="30" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="29" t="s">
+      <c r="A69" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="B69" s="29" t="s">
+      <c r="B69" s="30" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="29" t="s">
+      <c r="A70" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="B70" s="29" t="s">
+      <c r="B70" s="30" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="29" t="s">
+      <c r="A71" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="B71" s="29" t="s">
+      <c r="B71" s="30" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="29" t="s">
+      <c r="A72" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="B72" s="29" t="s">
+      <c r="B72" s="30" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="29" t="s">
+      <c r="A73" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="B73" s="29" t="s">
+      <c r="B73" s="30" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="29" t="s">
+      <c r="A74" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="B74" s="29" t="s">
+      <c r="B74" s="30" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="29" t="s">
+      <c r="A75" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="B75" s="29" t="s">
+      <c r="B75" s="30" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="29" t="s">
+      <c r="A76" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="B76" s="29" t="s">
+      <c r="B76" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="29" t="s">
+      <c r="A77" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="B77" s="29" t="s">
+      <c r="B77" s="30" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="29" t="s">
+      <c r="A78" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="B78" s="29" t="s">
+      <c r="B78" s="30" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="29" t="s">
+      <c r="A79" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="B79" s="29" t="s">
+      <c r="B79" s="30" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="29" t="s">
+      <c r="A80" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="B80" s="29" t="s">
+      <c r="B80" s="30" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="29" t="s">
+      <c r="A81" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="B81" s="29" t="s">
+      <c r="B81" s="30" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="29" t="s">
+      <c r="A82" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="B82" s="29" t="s">
+      <c r="B82" s="30" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="29" t="s">
+      <c r="A83" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="B83" s="29" t="s">
+      <c r="B83" s="30" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="29" t="s">
+      <c r="A84" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="B84" s="29" t="s">
+      <c r="B84" s="30" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="29" t="s">
+      <c r="A85" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="B85" s="29" t="s">
+      <c r="B85" s="30" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="29" t="s">
+      <c r="A86" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="B86" s="29" t="s">
+      <c r="B86" s="30" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="29" t="s">
+      <c r="A87" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="B87" s="29" t="s">
+      <c r="B87" s="30" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="29" t="s">
+      <c r="A88" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="B88" s="29" t="s">
+      <c r="B88" s="30" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="29" t="s">
+      <c r="A89" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="B89" s="29" t="s">
+      <c r="B89" s="30" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="29" t="s">
+      <c r="A90" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="B90" s="29" t="s">
+      <c r="B90" s="30" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="29" t="s">
+      <c r="A91" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="B91" s="29" t="s">
+      <c r="B91" s="30" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="29" t="s">
+      <c r="A92" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="B92" s="29" t="s">
+      <c r="B92" s="30" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="29" t="s">
+      <c r="A93" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="B93" s="29" t="s">
+      <c r="B93" s="30" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="29" t="s">
+      <c r="A94" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="B94" s="29" t="s">
+      <c r="B94" s="30" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="29" t="s">
+      <c r="A95" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="B95" s="29" t="s">
+      <c r="B95" s="30" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="29" t="s">
+      <c r="A96" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="B96" s="29" t="s">
+      <c r="B96" s="30" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="29" t="s">
+      <c r="A97" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="B97" s="29" t="s">
+      <c r="B97" s="30" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B98" s="29" t="s">
+      <c r="B98" s="30" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B99" s="29" t="s">
+      <c r="B99" s="30" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B100" s="29" t="s">
+      <c r="B100" s="30" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B101" s="29" t="s">
+      <c r="B101" s="30" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B102" s="29" t="s">
+      <c r="B102" s="30" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B103" s="29" t="s">
+      <c r="B103" s="30" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B104" s="29" t="s">
+      <c r="B104" s="30" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B105" s="29" t="s">
+      <c r="B105" s="30" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B106" s="29" t="s">
+      <c r="B106" s="30" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B107" s="29" t="s">
+      <c r="B107" s="30" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B108" s="29" t="s">
+      <c r="B108" s="30" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B109" s="29" t="s">
+      <c r="B109" s="30" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B110" s="29" t="s">
+      <c r="B110" s="30" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B111" s="29" t="s">
+      <c r="B111" s="30" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B112" s="29" t="s">
+      <c r="B112" s="30" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B113" s="29" t="s">
+      <c r="B113" s="30" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B114" s="29" t="s">
+      <c r="B114" s="30" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B115" s="29" t="s">
+      <c r="B115" s="30" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B116" s="29" t="s">
+      <c r="B116" s="30" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B117" s="29" t="s">
+      <c r="B117" s="30" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B118" s="29" t="s">
+      <c r="B118" s="30" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B119" s="29" t="s">
+      <c r="B119" s="30" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B120" s="29" t="s">
+      <c r="B120" s="30" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B121" s="29" t="s">
+      <c r="B121" s="30" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B122" s="29" t="s">
+      <c r="B122" s="30" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B123" s="29" t="s">
+      <c r="B123" s="30" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B124" s="29" t="s">
+      <c r="B124" s="30" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B125" s="29" t="s">
+      <c r="B125" s="30" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B126" s="29" t="s">
+      <c r="B126" s="30" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B127" s="29" t="s">
+      <c r="B127" s="30" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B128" s="29" t="s">
+      <c r="B128" s="30" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B129" s="29" t="s">
+      <c r="B129" s="30" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B130" s="29" t="s">
+      <c r="B130" s="30" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B131" s="29" t="s">
+      <c r="B131" s="30" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B132" s="29" t="s">
+      <c r="B132" s="30" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B133" s="29" t="s">
+      <c r="B133" s="30" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B134" s="29" t="s">
+      <c r="B134" s="30" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B135" s="29" t="s">
+      <c r="B135" s="30" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B136" s="29" t="s">
+      <c r="B136" s="30" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B137" s="29" t="s">
+      <c r="B137" s="30" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B138" s="29" t="s">
+      <c r="B138" s="30" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B139" s="29" t="s">
+      <c r="B139" s="30" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B140" s="29" t="s">
+      <c r="B140" s="30" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B141" s="29" t="s">
+      <c r="B141" s="30" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B142" s="29" t="s">
+      <c r="B142" s="30" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B143" s="29" t="s">
+      <c r="B143" s="30" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B144" s="29" t="s">
+      <c r="B144" s="30" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B145" s="29" t="s">
+      <c r="B145" s="30" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B146" s="29" t="s">
+      <c r="B146" s="30" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B147" s="29" t="s">
+      <c r="B147" s="30" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B148" s="29" t="s">
+      <c r="B148" s="30" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B149" s="29" t="s">
+      <c r="B149" s="30" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B150" s="29" t="s">
+      <c r="B150" s="30" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B151" s="29" t="s">
+      <c r="B151" s="30" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B152" s="29" t="s">
+      <c r="B152" s="30" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B153" s="29" t="s">
+      <c r="B153" s="30" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B154" s="29" t="s">
+      <c r="B154" s="30" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B155" s="29" t="s">
+      <c r="B155" s="30" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B156" s="29" t="s">
+      <c r="B156" s="30" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B157" s="29" t="s">
+      <c r="B157" s="30" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B158" s="29" t="s">
+      <c r="B158" s="30" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B159" s="29" t="s">
+      <c r="B159" s="30" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B160" s="29" t="s">
+      <c r="B160" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B161" s="29" t="s">
+      <c r="B161" s="30" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B162" s="29" t="s">
+      <c r="B162" s="30" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B163" s="29" t="s">
+      <c r="B163" s="30" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B164" s="29" t="s">
+      <c r="B164" s="30" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B165" s="29" t="s">
+      <c r="B165" s="30" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B166" s="29" t="s">
+      <c r="B166" s="30" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B167" s="29" t="s">
+      <c r="B167" s="30" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B168" s="29" t="s">
+      <c r="B168" s="30" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B169" s="29" t="s">
+      <c r="B169" s="30" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B170" s="29" t="s">
+      <c r="B170" s="30" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B171" s="29" t="s">
+      <c r="B171" s="30" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B172" s="29" t="s">
+      <c r="B172" s="30" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B173" s="29" t="s">
+      <c r="B173" s="30" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B174" s="29" t="s">
+      <c r="B174" s="30" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B175" s="29" t="s">
+      <c r="B175" s="30" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B176" s="29" t="s">
+      <c r="B176" s="30" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B177" s="29" t="s">
+      <c r="B177" s="30" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B178" s="29" t="s">
+      <c r="B178" s="30" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B179" s="29" t="s">
+      <c r="B179" s="30" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B180" s="29" t="s">
+      <c r="B180" s="30" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B181" s="29" t="s">
+      <c r="B181" s="30" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B182" s="29" t="s">
+      <c r="B182" s="30" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B183" s="29" t="s">
+      <c r="B183" s="30" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B184" s="29" t="s">
+      <c r="B184" s="30" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B185" s="29" t="s">
+      <c r="B185" s="30" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B186" s="29" t="s">
+      <c r="B186" s="30" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B187" s="29" t="s">
+      <c r="B187" s="30" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B188" s="29" t="s">
+      <c r="B188" s="30" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B189" s="29" t="s">
+      <c r="B189" s="30" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B190" s="29" t="s">
+      <c r="B190" s="30" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B191" s="29" t="s">
+      <c r="B191" s="30" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B192" s="29" t="s">
+      <c r="B192" s="30" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B193" s="29" t="s">
+      <c r="B193" s="30" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B194" s="29" t="s">
+      <c r="B194" s="30" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B195" s="29" t="s">
+      <c r="B195" s="30" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B196" s="29" t="s">
+      <c r="B196" s="30" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B197" s="29" t="s">
+      <c r="B197" s="30" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B198" s="29" t="s">
+      <c r="B198" s="30" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B199" s="29" t="s">
+      <c r="B199" s="30" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B200" s="29" t="s">
+      <c r="B200" s="30" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B201" s="29" t="s">
+      <c r="B201" s="30" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B202" s="29" t="s">
+      <c r="B202" s="30" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B203" s="29" t="s">
+      <c r="B203" s="30" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B204" s="29" t="s">
+      <c r="B204" s="30" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B205" s="29" t="s">
+      <c r="B205" s="30" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B206" s="29" t="s">
+      <c r="B206" s="30" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B207" s="29" t="s">
+      <c r="B207" s="30" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B208" s="29" t="s">
+      <c r="B208" s="30" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B209" s="29" t="s">
+      <c r="B209" s="30" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B210" s="29" t="s">
+      <c r="B210" s="30" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B211" s="29" t="s">
+      <c r="B211" s="30" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B212" s="29" t="s">
+      <c r="B212" s="30" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B213" s="29" t="s">
+      <c r="B213" s="30" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B214" s="29" t="s">
+      <c r="B214" s="30" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B215" s="29" t="s">
+      <c r="B215" s="30" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B216" s="29" t="s">
+      <c r="B216" s="30" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B217" s="29" t="s">
+      <c r="B217" s="30" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B218" s="29" t="s">
+      <c r="B218" s="30" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B219" s="29" t="s">
+      <c r="B219" s="30" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B220" s="29" t="s">
+      <c r="B220" s="30" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B221" s="29" t="s">
+      <c r="B221" s="30" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B222" s="29" t="s">
+      <c r="B222" s="30" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B223" s="29" t="s">
+      <c r="B223" s="30" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B224" s="29" t="s">
+      <c r="B224" s="30" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B225" s="29" t="s">
+      <c r="B225" s="30" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B226" s="29" t="s">
+      <c r="B226" s="30" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B227" s="29" t="s">
+      <c r="B227" s="30" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B228" s="29" t="s">
+      <c r="B228" s="30" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B229" s="29" t="s">
+      <c r="B229" s="30" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B230" s="29" t="s">
+      <c r="B230" s="30" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B231" s="29" t="s">
+      <c r="B231" s="30" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B232" s="29" t="s">
+      <c r="B232" s="30" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B233" s="29" t="s">
+      <c r="B233" s="30" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B234" s="29" t="s">
+      <c r="B234" s="30" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B235" s="29" t="s">
+      <c r="B235" s="30" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B236" s="29" t="s">
+      <c r="B236" s="30" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B237" s="29" t="s">
+      <c r="B237" s="30" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B238" s="29" t="s">
+      <c r="B238" s="30" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B239" s="29" t="s">
+      <c r="B239" s="30" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B240" s="29" t="s">
+      <c r="B240" s="30" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B241" s="29" t="s">
+      <c r="B241" s="30" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B242" s="29" t="s">
+      <c r="B242" s="30" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B243" s="29" t="s">
+      <c r="B243" s="30" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B244" s="29" t="s">
+      <c r="B244" s="30" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B245" s="29" t="s">
+      <c r="B245" s="30" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B246" s="29" t="s">
+      <c r="B246" s="30" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B247" s="29" t="s">
+      <c r="B247" s="30" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B248" s="29" t="s">
+      <c r="B248" s="30" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B249" s="29" t="s">
+      <c r="B249" s="30" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B250" s="29" t="s">
+      <c r="B250" s="30" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B251" s="29" t="s">
+      <c r="B251" s="30" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B252" s="29" t="s">
+      <c r="B252" s="30" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B253" s="29" t="s">
+      <c r="B253" s="30" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B254" s="29" t="s">
+      <c r="B254" s="30" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B255" s="29" t="s">
+      <c r="B255" s="30" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B256" s="29" t="s">
+      <c r="B256" s="30" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B257" s="29" t="s">
+      <c r="B257" s="30" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B258" s="29" t="s">
+      <c r="B258" s="30" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B259" s="29" t="s">
+      <c r="B259" s="30" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B260" s="29" t="s">
+      <c r="B260" s="30" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B261" s="29" t="s">
+      <c r="B261" s="30" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B262" s="29" t="s">
+      <c r="B262" s="30" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B263" s="29" t="s">
+      <c r="B263" s="30" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B264" s="29" t="s">
+      <c r="B264" s="30" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B265" s="29" t="s">
+      <c r="B265" s="30" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B266" s="29" t="s">
+      <c r="B266" s="30" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B267" s="29" t="s">
+      <c r="B267" s="30" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B268" s="29" t="s">
+      <c r="B268" s="30" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B269" s="29" t="s">
+      <c r="B269" s="30" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B270" s="29" t="s">
+      <c r="B270" s="30" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B271" s="29" t="s">
+      <c r="B271" s="30" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B272" s="29" t="s">
+      <c r="B272" s="30" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B273" s="29" t="s">
+      <c r="B273" s="30" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B274" s="29" t="s">
+      <c r="B274" s="30" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B275" s="29" t="s">
+      <c r="B275" s="30" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B276" s="29" t="s">
+      <c r="B276" s="30" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B277" s="29" t="s">
+      <c r="B277" s="30" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B278" s="29" t="s">
+      <c r="B278" s="30" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B279" s="29" t="s">
+      <c r="B279" s="30" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B280" s="29" t="s">
+      <c r="B280" s="30" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B281" s="29" t="s">
+      <c r="B281" s="30" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B282" s="29" t="s">
+      <c r="B282" s="30" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B283" s="29" t="s">
+      <c r="B283" s="30" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B284" s="29" t="s">
+      <c r="B284" s="30" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B285" s="29" t="s">
+      <c r="B285" s="30" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B286" s="29" t="s">
+      <c r="B286" s="30" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B287" s="29" t="s">
+      <c r="B287" s="30" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B288" s="29" t="s">
+      <c r="B288" s="30" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B289" s="29" t="s">
+      <c r="B289" s="30" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B290" s="29" t="s">
+      <c r="B290" s="30" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B291" s="29" t="s">
+      <c r="B291" s="30" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B292" s="29" t="s">
+      <c r="B292" s="30" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B293" s="29" t="s">
+      <c r="B293" s="30" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B294" s="29" t="s">
+      <c r="B294" s="30" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B295" s="29" t="s">
+      <c r="B295" s="30" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B296" s="29" t="s">
+      <c r="B296" s="30" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B297" s="29" t="s">
+      <c r="B297" s="30" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B298" s="29" t="s">
+      <c r="B298" s="30" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B299" s="29" t="s">
+      <c r="B299" s="30" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B300" s="29" t="s">
+      <c r="B300" s="30" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B301" s="29" t="s">
+      <c r="B301" s="30" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B302" s="29" t="s">
+      <c r="B302" s="30" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B303" s="29" t="s">
+      <c r="B303" s="30" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B304" s="29" t="s">
+      <c r="B304" s="30" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B305" s="29" t="s">
+      <c r="B305" s="30" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B306" s="29" t="s">
+      <c r="B306" s="30" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B307" s="29" t="s">
+      <c r="B307" s="30" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B308" s="29" t="s">
+      <c r="B308" s="30" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B309" s="29" t="s">
+      <c r="B309" s="30" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B310" s="29" t="s">
+      <c r="B310" s="30" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B311" s="29" t="s">
+      <c r="B311" s="30" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B312" s="29" t="s">
+      <c r="B312" s="30" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B313" s="29" t="s">
+      <c r="B313" s="30" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B314" s="29" t="s">
+      <c r="B314" s="30" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B315" s="29" t="s">
+      <c r="B315" s="30" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B316" s="29" t="s">
+      <c r="B316" s="30" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B317" s="29" t="s">
+      <c r="B317" s="30" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B318" s="29" t="s">
+      <c r="B318" s="30" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B319" s="29" t="s">
+      <c r="B319" s="30" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B320" s="29" t="s">
+      <c r="B320" s="30" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B321" s="29" t="s">
+      <c r="B321" s="30" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B322" s="29" t="s">
+      <c r="B322" s="30" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B323" s="29" t="s">
+      <c r="B323" s="30" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B324" s="29" t="s">
+      <c r="B324" s="30" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B325" s="29" t="s">
+      <c r="B325" s="30" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B326" s="29" t="s">
+      <c r="B326" s="30" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B327" s="29" t="s">
+      <c r="B327" s="30" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B328" s="29" t="s">
+      <c r="B328" s="30" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B329" s="29" t="s">
+      <c r="B329" s="30" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B330" s="29" t="s">
+      <c r="B330" s="30" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B331" s="29" t="s">
+      <c r="B331" s="30" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B332" s="29" t="s">
+      <c r="B332" s="30" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B333" s="29" t="s">
+      <c r="B333" s="30" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B334" s="29" t="s">
+      <c r="B334" s="30" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B335" s="29" t="s">
+      <c r="B335" s="30" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B336" s="29" t="s">
+      <c r="B336" s="30" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B337" s="29" t="s">
+      <c r="B337" s="30" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B338" s="29" t="s">
+      <c r="B338" s="30" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B339" s="29" t="s">
+      <c r="B339" s="30" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B340" s="29" t="s">
+      <c r="B340" s="30" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B341" s="29" t="s">
+      <c r="B341" s="30" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B342" s="29" t="s">
+      <c r="B342" s="30" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B343" s="29" t="s">
+      <c r="B343" s="30" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B344" s="29" t="s">
+      <c r="B344" s="30" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B345" s="29" t="s">
+      <c r="B345" s="30" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B346" s="29" t="s">
+      <c r="B346" s="30" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B347" s="29" t="s">
+      <c r="B347" s="30" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B348" s="29" t="s">
+      <c r="B348" s="30" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B349" s="29" t="s">
+      <c r="B349" s="30" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B350" s="29" t="s">
+      <c r="B350" s="30" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B351" s="29" t="s">
+      <c r="B351" s="30" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B352" s="29" t="s">
+      <c r="B352" s="30" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B353" s="29" t="s">
+      <c r="B353" s="30" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B354" s="29" t="s">
+      <c r="B354" s="30" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B355" s="29" t="s">
+      <c r="B355" s="30" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B356" s="29" t="s">
+      <c r="B356" s="30" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B357" s="29" t="s">
+      <c r="B357" s="30" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B358" s="29" t="s">
+      <c r="B358" s="30" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B359" s="29" t="s">
+      <c r="B359" s="30" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B360" s="29" t="s">
+      <c r="B360" s="30" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B361" s="29" t="s">
+      <c r="B361" s="30" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B362" s="29" t="s">
+      <c r="B362" s="30" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B363" s="29" t="s">
+      <c r="B363" s="30" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B364" s="29" t="s">
+      <c r="B364" s="30" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B365" s="29" t="s">
+      <c r="B365" s="30" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B366" s="29" t="s">
+      <c r="B366" s="30" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B367" s="29" t="s">
+      <c r="B367" s="30" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B368" s="29" t="s">
+      <c r="B368" s="30" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B369" s="29" t="s">
+      <c r="B369" s="30" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B370" s="29" t="s">
+      <c r="B370" s="30" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B371" s="29" t="s">
+      <c r="B371" s="30" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B372" s="29" t="s">
+      <c r="B372" s="30" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B373" s="29" t="s">
+      <c r="B373" s="30" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B374" s="29" t="s">
+      <c r="B374" s="30" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B375" s="29" t="s">
+      <c r="B375" s="30" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B376" s="29" t="s">
+      <c r="B376" s="30" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B377" s="29" t="s">
+      <c r="B377" s="30" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B378" s="29" t="s">
+      <c r="B378" s="30" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B379" s="29" t="s">
+      <c r="B379" s="30" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B380" s="29" t="s">
+      <c r="B380" s="30" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B381" s="29" t="s">
+      <c r="B381" s="30" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B382" s="29" t="s">
+      <c r="B382" s="30" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B383" s="29" t="s">
+      <c r="B383" s="30" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B384" s="29" t="s">
+      <c r="B384" s="30" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B385" s="29" t="s">
+      <c r="B385" s="30" t="s">
         <v>427</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix most remaining issues.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_QC_v4_1_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_QC_v4_1_0.xlsx
@@ -1763,7 +1763,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.88"/>
@@ -6809,7 +6809,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.5"/>
@@ -6873,10 +6873,11 @@
       </c>
       <c r="G2" s="30"/>
       <c r="H2" s="31" t="n">
-        <v>607.558</v>
+        <v>617.9</v>
       </c>
       <c r="I2" s="31" t="n">
-        <v>303.779</v>
+        <f aca="false">H2/2</f>
+        <v>308.95</v>
       </c>
       <c r="J2" s="30"/>
       <c r="K2" s="30" t="s">

</xml_diff>